<commit_message>
Correction on ihr and ifr column order
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_v18.xlsx
+++ b/Template_CoMoCOVID-19App_v18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23485AA1-A9AD-9842-91DF-AE48098FB734}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C09C12-BA0C-A646-A980-4FFDDA43686A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1740" yWindow="-19280" windowWidth="27320" windowHeight="16000" tabRatio="648" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27880" windowHeight="17500" tabRatio="648" activeTab="2" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -3418,7 +3418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3677,32 +3677,15 @@
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3747,6 +3730,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3761,14 +3754,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F16" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="E1:F16" xr:uid="{2E89BE7F-E667-6946-928D-DC5AB4119A65}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F8">
     <sortCondition ref="E1:E8"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4074,7 +4067,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6394,7 +6387,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F100">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>NOT(OR($A2 = "Vaccination", $A2 = "School Closures", $A2 = "Partial School Closures",  $A2 = "Mass Testing"))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8492,8 +8485,8 @@
   </sheetPr>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -8519,236 +8512,236 @@
       <c r="A2" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="B2" s="76">
+      <c r="B2" s="112">
+        <v>0.6</v>
+      </c>
+      <c r="C2" s="112">
         <v>0.1</v>
-      </c>
-      <c r="C2" s="76">
-        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="112">
+        <v>0.6</v>
+      </c>
+      <c r="C3" s="112">
         <v>0.1</v>
-      </c>
-      <c r="C3" s="76">
-        <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="76">
+      <c r="B4" s="112">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="112">
         <v>0.1</v>
-      </c>
-      <c r="C4" s="76">
-        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="112">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="112">
         <v>0.1</v>
-      </c>
-      <c r="C5" s="76">
-        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="112">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C6" s="112">
         <v>0.5</v>
-      </c>
-      <c r="C6" s="76">
-        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="112">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C7" s="112">
         <v>0.5</v>
-      </c>
-      <c r="C7" s="76">
-        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="76">
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="C8" s="76">
+      <c r="B8" s="112">
         <v>1.9</v>
+      </c>
+      <c r="C8" s="112">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="76">
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="C9" s="76">
+      <c r="B9" s="112">
         <v>1.9</v>
+      </c>
+      <c r="C9" s="112">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="76">
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="C10" s="76">
-        <v>3.3000000000000003</v>
+      <c r="B10" s="112">
+        <v>3.3</v>
+      </c>
+      <c r="C10" s="112">
+        <v>1.4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="76">
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="C11" s="76">
-        <v>3.3000000000000003</v>
+      <c r="B11" s="112">
+        <v>3.3</v>
+      </c>
+      <c r="C11" s="112">
+        <v>1.4</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="76">
-        <v>2.9000000000000004</v>
-      </c>
-      <c r="C12" s="76">
+      <c r="B12" s="112">
         <v>6.5</v>
+      </c>
+      <c r="C12" s="112">
+        <v>2.9</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="76">
-        <v>2.9000000000000004</v>
-      </c>
-      <c r="C13" s="76">
+      <c r="B13" s="112">
         <v>6.5</v>
+      </c>
+      <c r="C13" s="112">
+        <v>2.9</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="76">
-        <v>5.8000000000000007</v>
-      </c>
-      <c r="C14" s="76">
+      <c r="B14" s="112">
         <v>12.6</v>
+      </c>
+      <c r="C14" s="112">
+        <v>5.8</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="76">
-        <v>5.8000000000000007</v>
-      </c>
-      <c r="C15" s="76">
+      <c r="B15" s="112">
         <v>12.6</v>
+      </c>
+      <c r="C15" s="112">
+        <v>5.8</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="76">
+      <c r="B16" s="112">
+        <v>21</v>
+      </c>
+      <c r="C16" s="112">
         <v>9.3000000000000007</v>
-      </c>
-      <c r="C16" s="76">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="76">
+      <c r="B17" s="112">
+        <v>21</v>
+      </c>
+      <c r="C17" s="112">
         <v>9.3000000000000007</v>
-      </c>
-      <c r="C17" s="76">
-        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="76">
-        <v>26.200000000000003</v>
-      </c>
-      <c r="C18" s="76">
+      <c r="B18" s="112">
         <v>31.6</v>
+      </c>
+      <c r="C18" s="112">
+        <v>26.2</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="76">
-        <v>26.200000000000003</v>
-      </c>
-      <c r="C19" s="76">
+      <c r="B19" s="112">
         <v>31.6</v>
+      </c>
+      <c r="C19" s="112">
+        <v>26.2</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="76">
-        <v>26.200000000000003</v>
-      </c>
-      <c r="C20" s="76">
+      <c r="B20" s="112">
         <v>31.6</v>
+      </c>
+      <c r="C20" s="112">
+        <v>26.2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="76">
-        <v>26.200000000000003</v>
-      </c>
-      <c r="C21" s="76">
+      <c r="B21" s="112">
         <v>31.6</v>
+      </c>
+      <c r="C21" s="112">
+        <v>26.2</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="76">
-        <v>26.200000000000003</v>
-      </c>
-      <c r="C22" s="76">
+      <c r="B22" s="112">
         <v>31.6</v>
+      </c>
+      <c r="C22" s="112">
+        <v>26.2</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2:C22" xr:uid="{6F77CD72-3BB7-4451-8487-AA34D9320359}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2:C22" xr:uid="{6764B28F-EEAB-5F4A-838F-FD36DD7F6B03}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Ricardo fix for sigma
</commit_message>
<xml_diff>
--- a/Template_CoMoCOVID-19App_v18.xlsx
+++ b/Template_CoMoCOVID-19App_v18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/Documents/Projets/CoMo/como/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricardo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C09C12-BA0C-A646-A980-4FFDDA43686A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A3B205-F1C4-46C9-AD65-593F644CD0C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27880" windowHeight="17500" tabRatio="648" activeTab="2" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="648" activeTab="2" xr2:uid="{25C8D176-4C08-9D40-9B57-F7F8CA55C35B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,14 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -2773,7 +2781,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Change in probability of requiring hospitalisation if previously vaccinated</t>
+      <t xml:space="preserve">Days from seropositve to seronegative </t>
     </r>
   </si>
   <si>
@@ -2783,16 +2791,15 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t xml:space="preserve">(Prev. in Virus Param) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Change in probability of requiring hospitalisation if previously infected</t>
+      <t xml:space="preserve">(Optional Vaccine Formula) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Observed efficacy against disease (e.g. in a trial with a disease endpoint)</t>
     </r>
   </si>
   <si>
@@ -2802,16 +2809,25 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>(Prev. in Virus Param)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Change in probability of requiring hospitalisation if previously infected and vaccinated</t>
+      <t xml:space="preserve">(Optional Vaccine Formula) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fficacy against infection</t>
     </r>
   </si>
   <si>
@@ -2821,16 +2837,17 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t xml:space="preserve">(Prev. in Virus Param) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Days from seropositve to seronegative </t>
+      <t>(Optional Vaccine Formula)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Efficacy against disease given already infected</t>
     </r>
   </si>
   <si>
@@ -2840,15 +2857,36 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
+      <t>(Optional Vaccine Formula)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Efficacy against severe disease given already infected and has disease</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
       <t xml:space="preserve">(Optional Vaccine Formula) </t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Observed efficacy against disease (e.g. in a trial with a disease endpoint)</t>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Probability upon infection of developing clinical symptoms if previously vaccinated</t>
     </r>
   </si>
   <si>
@@ -2858,25 +2896,16 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t xml:space="preserve">(Optional Vaccine Formula) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fficacy against infection</t>
+      <t>(Prev. in Virus Param)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Probability upon infection of developing clinical symptoms if previously vaccinated</t>
     </r>
   </si>
   <si>
@@ -2886,17 +2915,64 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>(Optional Vaccine Formula)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Efficacy against disease given already infected</t>
+      <t xml:space="preserve">(Prev. in Interventions Param) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Vaccination - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Time to reach target coverage (1 to 52)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">(Prev. in Interventions Param) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vaccination - Duration of efficacious period</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">(Prev. in Interventions Param) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vaccination -  Duration of efficacious period if previously infected</t>
     </r>
   </si>
   <si>
@@ -2906,17 +2982,17 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>(Optional Vaccine Formula)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Efficacy against severe disease given already infected and has disease</t>
+      <t>(Prev. in Interventions Param)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vaccination -  Efficacy against infection</t>
     </r>
   </si>
   <si>
@@ -2926,17 +3002,50 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t xml:space="preserve">(Optional Vaccine Formula) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Probability upon infection of developing clinical symptoms if previously vaccinated</t>
-    </r>
+      <t xml:space="preserve">(Prev. in Interventions Param) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">Vaccination -  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Efficacy against infection if previously infected</t>
+    </r>
+  </si>
+  <si>
+    <t>You can inform the vaccine related model parameters by filling in the yellow cells. These values should be taken directly from the published efficacies against infection and disease generated by the vaccine clinical trials</t>
+  </si>
+  <si>
+    <t>All Vaccination Parameters have been regrouped into the "Vaccination Param" sheet and several formulas have been addded.</t>
+  </si>
+  <si>
+    <t>Partial School Closures</t>
+  </si>
+  <si>
+    <t>Template v18</t>
+  </si>
+  <si>
+    <t>New in v18</t>
+  </si>
+  <si>
+    <t>Added a "Partial School Closures" intervention.</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>v18.a</t>
   </si>
   <si>
     <r>
@@ -2954,7 +3063,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Change in probability of requiring hospitalisation if previously vaccinated</t>
+      <t>Probability of requiring hospitalisation if previously vaccinated</t>
     </r>
   </si>
   <si>
@@ -2964,16 +3073,16 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>(Prev. in Virus Param)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Probability upon infection of developing clinical symptoms if previously vaccinated</t>
+      <t xml:space="preserve">(Prev. in Virus Param) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Probability of requiring hospitalisation if previously vaccinated</t>
     </r>
   </si>
   <si>
@@ -2983,64 +3092,16 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t xml:space="preserve">(Prev. in Interventions Param) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">Vaccination - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Time to reach target coverage (1 to 52)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">(Prev. in Interventions Param) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vaccination - Duration of efficacious period</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">(Prev. in Interventions Param) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vaccination -  Duration of efficacious period if previously infected</t>
+      <t xml:space="preserve">(Prev. in Virus Param) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Probability of requiring hospitalisation if previously infected</t>
     </r>
   </si>
   <si>
@@ -3050,70 +3111,17 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>(Prev. in Interventions Param)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Vaccination -  Efficacy against infection</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">(Prev. in Interventions Param) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t xml:space="preserve">Vaccination -  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Efficacy against infection if previously infected</t>
-    </r>
-  </si>
-  <si>
-    <t>You can inform the vaccine related model parameters by filling in the yellow cells. These values should be taken directly from the published efficacies against infection and disease generated by the vaccine clinical trials</t>
-  </si>
-  <si>
-    <t>All Vaccination Parameters have been regrouped into the "Vaccination Param" sheet and several formulas have been addded.</t>
-  </si>
-  <si>
-    <t>Partial School Closures</t>
-  </si>
-  <si>
-    <t>Template v18</t>
-  </si>
-  <si>
-    <t>New in v18</t>
-  </si>
-  <si>
-    <t>Added a "Partial School Closures" intervention.</t>
-  </si>
-  <si>
-    <t>1-2</t>
-  </si>
-  <si>
-    <t>v18.a</t>
+      <t>(Prev. in Virus Param)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Probability of requiring hospitalisation if previously infected and vaccinated</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3687,6 +3695,16 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3730,16 +3748,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3754,14 +3762,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F16" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB0B0E91-77B9-BF40-854E-551FE7298B58}" name="Table2" displayName="Table2" ref="E1:F16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="E1:F16" xr:uid="{2E89BE7F-E667-6946-928D-DC5AB4119A65}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F8">
     <sortCondition ref="E1:E8"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1DFAD25E-CC0B-354F-8701-442A29A91782}" name="Intervention" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D399EFFD-3A23-4943-B9C5-CF90FE06EA91}" name="Unit Intervention" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4071,17 +4079,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B1" s="91" t="s">
         <v>490</v>
-      </c>
-      <c r="B1" s="91" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="21">
@@ -4106,17 +4114,17 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="58" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="17">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="38" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="34">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="31.5">
       <c r="A9" s="38" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4124,7 +4132,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="89" customHeight="1">
+    <row r="12" spans="1:2" ht="89.1" customHeight="1">
       <c r="A12" s="38" t="s">
         <v>447</v>
       </c>
@@ -4285,27 +4293,27 @@
         <v>445</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="34">
+    <row r="42" spans="1:6" ht="31.5">
       <c r="A42" s="84" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="34">
+    <row r="43" spans="1:6" ht="31.5">
       <c r="A43" s="85" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="34">
+    <row r="44" spans="1:6" ht="31.5">
       <c r="A44" s="85" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17">
+    <row r="45" spans="1:6">
       <c r="A45" s="85" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="17">
+    <row r="46" spans="1:6">
       <c r="A46" s="85" t="s">
         <v>461</v>
       </c>
@@ -4318,27 +4326,27 @@
         <v>373</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="34">
+    <row r="50" spans="1:1" ht="31.5">
       <c r="A50" s="38" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="17">
+    <row r="51" spans="1:1">
       <c r="A51" s="38" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="17">
+    <row r="52" spans="1:1">
       <c r="A52" s="38" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="17">
+    <row r="53" spans="1:1">
       <c r="A53" s="38" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="34">
+    <row r="54" spans="1:1" ht="31.5">
       <c r="A54" s="38" t="s">
         <v>416</v>
       </c>
@@ -4363,17 +4371,17 @@
         <v>307</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="34">
+    <row r="61" spans="1:1" ht="31.5">
       <c r="A61" s="38" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="34">
+    <row r="62" spans="1:1" ht="31.5">
       <c r="A62" s="38" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="68">
+    <row r="63" spans="1:1" ht="63">
       <c r="A63" s="38" t="s">
         <v>340</v>
       </c>
@@ -4417,18 +4425,18 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="8.375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="8"/>
-    <col min="6" max="6" width="20.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>63</v>
       </c>
@@ -4458,7 +4466,7 @@
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
     </row>
-    <row r="3" spans="1:6" ht="18" thickBot="1">
+    <row r="3" spans="1:6" ht="16.5" thickBot="1">
       <c r="A3" s="15"/>
       <c r="B3" s="33" t="s">
         <v>74</v>
@@ -4486,7 +4494,7 @@
       <c r="E4" s="25"/>
       <c r="F4" s="26"/>
     </row>
-    <row r="5" spans="1:6" ht="17">
+    <row r="5" spans="1:6">
       <c r="A5" s="18"/>
       <c r="B5" s="35" t="s">
         <v>288</v>
@@ -4502,7 +4510,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" thickBot="1">
+    <row r="6" spans="1:6" ht="16.5" thickBot="1">
       <c r="A6" s="18"/>
       <c r="B6" s="35" t="s">
         <v>281</v>
@@ -4530,7 +4538,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="26"/>
     </row>
-    <row r="8" spans="1:6" ht="17">
+    <row r="8" spans="1:6">
       <c r="A8" s="15"/>
       <c r="B8" s="33" t="s">
         <v>86</v>
@@ -4548,7 +4556,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34">
+    <row r="9" spans="1:6" ht="31.5">
       <c r="A9" s="15"/>
       <c r="B9" s="35" t="s">
         <v>289</v>
@@ -4566,7 +4574,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34">
+    <row r="10" spans="1:6" ht="31.5">
       <c r="A10" s="15"/>
       <c r="B10" s="33" t="s">
         <v>87</v>
@@ -4584,7 +4592,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="35" thickBot="1">
+    <row r="11" spans="1:6" ht="32.25" thickBot="1">
       <c r="A11" s="21"/>
       <c r="B11" s="36" t="s">
         <v>88</v>
@@ -4612,7 +4620,7 @@
       <c r="E12" s="25"/>
       <c r="F12" s="26"/>
     </row>
-    <row r="13" spans="1:6" ht="18" thickBot="1">
+    <row r="13" spans="1:6" ht="16.5" thickBot="1">
       <c r="A13" s="46"/>
       <c r="B13" s="47" t="s">
         <v>74</v>
@@ -4640,7 +4648,7 @@
       <c r="E14" s="25"/>
       <c r="F14" s="26"/>
     </row>
-    <row r="15" spans="1:6" ht="18" thickBot="1">
+    <row r="15" spans="1:6" ht="16.5" thickBot="1">
       <c r="A15" s="46"/>
       <c r="B15" s="50" t="s">
         <v>284</v>
@@ -4668,7 +4676,7 @@
       <c r="E16" s="25"/>
       <c r="F16" s="26"/>
     </row>
-    <row r="17" spans="1:6" ht="18" thickBot="1">
+    <row r="17" spans="1:6" ht="16.5" thickBot="1">
       <c r="A17" s="46"/>
       <c r="B17" s="51" t="s">
         <v>331</v>
@@ -4696,7 +4704,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
     </row>
-    <row r="19" spans="1:6" ht="17">
+    <row r="19" spans="1:6">
       <c r="A19" s="53"/>
       <c r="B19" s="50" t="s">
         <v>75</v>
@@ -4714,7 +4722,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="35" thickBot="1">
+    <row r="20" spans="1:6" ht="32.25" thickBot="1">
       <c r="A20" s="46"/>
       <c r="B20" s="47" t="s">
         <v>76</v>
@@ -4742,7 +4750,7 @@
       <c r="E21" s="25"/>
       <c r="F21" s="26"/>
     </row>
-    <row r="22" spans="1:6" ht="18" thickBot="1">
+    <row r="22" spans="1:6" ht="16.5" thickBot="1">
       <c r="A22" s="46"/>
       <c r="B22" s="47" t="s">
         <v>78</v>
@@ -4770,7 +4778,7 @@
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
     </row>
-    <row r="24" spans="1:6" ht="17">
+    <row r="24" spans="1:6">
       <c r="A24" s="53"/>
       <c r="B24" s="50" t="s">
         <v>75</v>
@@ -4788,7 +4796,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18" thickBot="1">
+    <row r="25" spans="1:6" ht="16.5" thickBot="1">
       <c r="A25" s="46"/>
       <c r="B25" s="47" t="s">
         <v>290</v>
@@ -4816,7 +4824,7 @@
       <c r="E26" s="25"/>
       <c r="F26" s="26"/>
     </row>
-    <row r="27" spans="1:6" ht="17">
+    <row r="27" spans="1:6">
       <c r="A27" s="53"/>
       <c r="B27" s="50" t="s">
         <v>299</v>
@@ -4834,7 +4842,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="18" thickBot="1">
+    <row r="28" spans="1:6" ht="16.5" thickBot="1">
       <c r="A28" s="53"/>
       <c r="B28" s="50" t="s">
         <v>298</v>
@@ -4862,7 +4870,7 @@
       <c r="E29" s="25"/>
       <c r="F29" s="26"/>
     </row>
-    <row r="30" spans="1:6" ht="34">
+    <row r="30" spans="1:6" ht="31.5">
       <c r="A30" s="53"/>
       <c r="B30" s="51" t="s">
         <v>321</v>
@@ -4880,7 +4888,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="34">
+    <row r="31" spans="1:6" ht="31.5">
       <c r="A31" s="13"/>
       <c r="B31" s="51" t="s">
         <v>323</v>
@@ -4898,7 +4906,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="34">
+    <row r="32" spans="1:6" ht="31.5">
       <c r="A32" s="53"/>
       <c r="B32" s="51" t="s">
         <v>417</v>
@@ -4916,7 +4924,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="34">
+    <row r="33" spans="1:6" ht="31.5">
       <c r="A33" s="53"/>
       <c r="B33" s="50" t="s">
         <v>326</v>
@@ -4934,7 +4942,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" thickBot="1">
+    <row r="34" spans="1:6" ht="16.5" thickBot="1">
       <c r="A34" s="46"/>
       <c r="B34" s="47" t="s">
         <v>328</v>
@@ -5006,19 +5014,19 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="24.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>269</v>
       </c>
@@ -5355,7 +5363,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B16" s="7">
         <v>43983</v>
@@ -5371,7 +5379,7 @@
         <v>%</v>
       </c>
       <c r="F16" s="82" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>278</v>
@@ -6387,7 +6395,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F100">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(OR($A2 = "Vaccination", $A2 = "School Closures", $A2 = "Partial School Closures",  $A2 = "Mass Testing"))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6428,12 +6436,12 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="39.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="10.875" style="2"/>
+    <col min="5" max="5" width="39.875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6613,7 +6621,7 @@
         <v>126</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>31</v>
@@ -7328,18 +7336,18 @@
   <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="3" width="11" style="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="68">
+    <row r="1" spans="1:4" ht="63">
       <c r="A1" s="9" t="s">
         <v>280</v>
       </c>
@@ -8486,18 +8494,18 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C22"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="19.75" style="8" customWidth="1"/>
     <col min="4" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="170">
+    <row r="1" spans="1:3" ht="126" customHeight="1">
       <c r="A1" s="73" t="s">
         <v>279</v>
       </c>
@@ -8740,7 +8748,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2:C22" xr:uid="{6764B28F-EEAB-5F4A-838F-FD36DD7F6B03}">
       <formula1>0</formula1>
       <formula2>100</formula2>
@@ -8761,17 +8769,17 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="9" customWidth="1"/>
     <col min="4" max="5" width="11" style="9"/>
-    <col min="6" max="6" width="11.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="68">
+    <row r="1" spans="1:4" ht="63">
       <c r="A1" s="9" t="s">
         <v>279</v>
       </c>
@@ -9100,18 +9108,18 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="8"/>
+    <col min="7" max="16384" width="10.875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9134,7 +9142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17">
+    <row r="2" spans="1:6">
       <c r="A2" s="63" t="s">
         <v>398</v>
       </c>
@@ -9150,7 +9158,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17">
+    <row r="3" spans="1:6">
       <c r="A3" s="63" t="s">
         <v>399</v>
       </c>
@@ -9166,7 +9174,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17">
+    <row r="4" spans="1:6">
       <c r="A4" s="63" t="s">
         <v>452</v>
       </c>
@@ -9184,7 +9192,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="69" customFormat="1" ht="17">
+    <row r="5" spans="1:6" s="69" customFormat="1">
       <c r="A5" s="63" t="s">
         <v>374</v>
       </c>
@@ -9202,7 +9210,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17">
+    <row r="6" spans="1:6">
       <c r="A6" s="63" t="s">
         <v>397</v>
       </c>
@@ -9218,7 +9226,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17">
+    <row r="7" spans="1:6">
       <c r="A7" s="63" t="s">
         <v>396</v>
       </c>
@@ -9236,7 +9244,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17">
+    <row r="8" spans="1:6">
       <c r="A8" s="63" t="s">
         <v>395</v>
       </c>
@@ -9254,7 +9262,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17">
+    <row r="9" spans="1:6">
       <c r="A9" s="63" t="s">
         <v>394</v>
       </c>
@@ -9272,7 +9280,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17">
+    <row r="10" spans="1:6">
       <c r="A10" s="63" t="s">
         <v>451</v>
       </c>
@@ -9290,7 +9298,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17">
+    <row r="11" spans="1:6">
       <c r="A11" s="63" t="s">
         <v>393</v>
       </c>
@@ -9308,7 +9316,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34">
+    <row r="12" spans="1:6" ht="31.5">
       <c r="A12" s="63" t="s">
         <v>392</v>
       </c>
@@ -9326,7 +9334,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="34">
+    <row r="13" spans="1:6" ht="31.5">
       <c r="A13" s="63" t="s">
         <v>391</v>
       </c>
@@ -9344,7 +9352,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="34">
+    <row r="14" spans="1:6" ht="31.5">
       <c r="A14" s="63" t="s">
         <v>390</v>
       </c>
@@ -9362,7 +9370,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34">
+    <row r="15" spans="1:6" ht="31.5">
       <c r="A15" s="63" t="s">
         <v>389</v>
       </c>
@@ -9380,7 +9388,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="34">
+    <row r="16" spans="1:6" ht="31.5">
       <c r="A16" s="63" t="s">
         <v>388</v>
       </c>
@@ -9398,7 +9406,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34">
+    <row r="17" spans="1:6" ht="31.5">
       <c r="A17" s="63" t="s">
         <v>387</v>
       </c>
@@ -9416,7 +9424,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34">
+    <row r="18" spans="1:6" ht="31.5">
       <c r="A18" s="63" t="s">
         <v>375</v>
       </c>
@@ -9434,7 +9442,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="34">
+    <row r="19" spans="1:6" ht="31.5">
       <c r="A19" s="63" t="s">
         <v>376</v>
       </c>
@@ -9452,7 +9460,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="34">
+    <row r="20" spans="1:6" ht="31.5">
       <c r="A20" s="63" t="s">
         <v>377</v>
       </c>
@@ -9470,7 +9478,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17">
+    <row r="21" spans="1:6">
       <c r="A21" s="68" t="s">
         <v>341</v>
       </c>
@@ -9486,7 +9494,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17">
+    <row r="22" spans="1:6">
       <c r="A22" s="68" t="s">
         <v>303</v>
       </c>
@@ -9502,7 +9510,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17">
+    <row r="23" spans="1:6">
       <c r="A23" s="68" t="s">
         <v>304</v>
       </c>
@@ -9584,14 +9592,14 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="38.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="8" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
@@ -9702,14 +9710,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="66.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11" style="8"/>
-    <col min="6" max="6" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="8"/>
+    <col min="6" max="6" width="7.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="8"/>
     <col min="8" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
@@ -9730,7 +9738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17">
+    <row r="2" spans="1:5">
       <c r="A2" s="71" t="s">
         <v>378</v>
       </c>
@@ -9747,7 +9755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17">
+    <row r="3" spans="1:5">
       <c r="A3" s="71" t="s">
         <v>379</v>
       </c>
@@ -9764,7 +9772,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17">
+    <row r="4" spans="1:5">
       <c r="A4" s="71" t="s">
         <v>380</v>
       </c>
@@ -9781,7 +9789,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17">
+    <row r="5" spans="1:5">
       <c r="A5" s="71" t="s">
         <v>381</v>
       </c>
@@ -9796,7 +9804,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17">
+    <row r="6" spans="1:5">
       <c r="A6" s="71" t="s">
         <v>382</v>
       </c>
@@ -9813,7 +9821,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17">
+    <row r="7" spans="1:5">
       <c r="A7" s="71" t="s">
         <v>383</v>
       </c>
@@ -9830,7 +9838,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17">
+    <row r="8" spans="1:5">
       <c r="A8" s="71" t="s">
         <v>384</v>
       </c>
@@ -9847,7 +9855,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17">
+    <row r="9" spans="1:5">
       <c r="A9" s="71" t="s">
         <v>385</v>
       </c>
@@ -9864,7 +9872,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17">
+    <row r="10" spans="1:5">
       <c r="A10" s="71" t="s">
         <v>386</v>
       </c>
@@ -9881,7 +9889,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17">
+    <row r="11" spans="1:5">
       <c r="A11" s="71" t="s">
         <v>305</v>
       </c>
@@ -9901,7 +9909,7 @@
     <row r="20" s="70" customFormat="1"/>
     <row r="21" s="70" customFormat="1" ht="30" customHeight="1"/>
     <row r="22" s="70" customFormat="1" ht="32.25" customHeight="1"/>
-    <row r="23" s="70" customFormat="1" ht="17" customHeight="1"/>
+    <row r="23" s="70" customFormat="1" ht="17.100000000000001" customHeight="1"/>
     <row r="24" s="70" customFormat="1"/>
     <row r="25" s="70" customFormat="1"/>
   </sheetData>
@@ -9946,13 +9954,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="71.5" style="8" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
@@ -10360,16 +10368,16 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="104.33203125" style="60" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="8"/>
-    <col min="5" max="5" width="15.6640625" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="104.375" style="60" customWidth="1"/>
+    <col min="2" max="2" width="5.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.875" style="8"/>
+    <col min="5" max="5" width="15.625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10391,7 +10399,7 @@
     </row>
     <row r="2" spans="1:5" ht="41.25" customHeight="1">
       <c r="A2" s="111" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -10400,7 +10408,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="110" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B3" s="99">
         <v>80</v>
@@ -10411,7 +10419,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="60" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B4" s="99">
         <v>20</v>
@@ -10422,7 +10430,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="60" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B5" s="100">
         <f>100*(1-((1-B3/100)/(1-B4/100)))</f>
@@ -10434,7 +10442,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="60" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B6" s="99">
         <v>50</v>
@@ -10443,9 +10451,9 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="17">
+    <row r="7" spans="1:5">
       <c r="A7" s="101" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B7" s="100">
         <f>'Virus Param'!B8*(1-B3/100)/(1-B4/100)</f>
@@ -10455,13 +10463,13 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" s="69" customFormat="1" ht="17">
+    <row r="8" spans="1:5" s="69" customFormat="1">
       <c r="A8" s="101" t="s">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="B8" s="100">
-        <f>100*(1-(B7/'Virus Param'!B8)*(1-'Vaccination Param'!B6/100))</f>
-        <v>87.5</v>
+        <f>100-100*(1-(B7/'Virus Param'!B8)*(1-'Vaccination Param'!B6/100))</f>
+        <v>12.5</v>
       </c>
       <c r="C8" s="96"/>
       <c r="D8" s="96"/>
@@ -10474,9 +10482,9 @@
       <c r="D9" s="96"/>
       <c r="E9" s="96"/>
     </row>
-    <row r="10" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="10" spans="1:5" s="60" customFormat="1">
       <c r="A10" s="101" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B10" s="102">
         <f>$B$7</f>
@@ -10492,7 +10500,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="11" spans="1:5" s="60" customFormat="1">
       <c r="A11" s="101" t="s">
         <v>462</v>
       </c>
@@ -10510,7 +10518,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="12" spans="1:5" s="60" customFormat="1">
       <c r="A12" s="101" t="s">
         <v>463</v>
       </c>
@@ -10528,7 +10536,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="13" spans="1:5" s="60" customFormat="1">
       <c r="A13" s="101" t="s">
         <v>464</v>
       </c>
@@ -10546,7 +10554,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="14" spans="1:5" s="60" customFormat="1">
       <c r="A14" s="101" t="s">
         <v>465</v>
       </c>
@@ -10564,7 +10572,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="15" spans="1:5" s="60" customFormat="1">
       <c r="A15" s="101" t="s">
         <v>466</v>
       </c>
@@ -10582,7 +10590,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="16" spans="1:5" s="60" customFormat="1">
       <c r="A16" s="101" t="s">
         <v>467</v>
       </c>
@@ -10600,7 +10608,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="17" spans="1:5" s="60" customFormat="1">
       <c r="A17" s="101" t="s">
         <v>468</v>
       </c>
@@ -10618,7 +10626,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="18" spans="1:5" s="60" customFormat="1">
       <c r="A18" s="101" t="s">
         <v>469</v>
       </c>
@@ -10636,7 +10644,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="60" customFormat="1" ht="17">
+    <row r="19" spans="1:5" s="60" customFormat="1">
       <c r="A19" s="105" t="s">
         <v>470</v>
       </c>
@@ -10653,13 +10661,13 @@
         <v>365</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="20" spans="1:5" s="30" customFormat="1">
       <c r="A20" s="93" t="s">
-        <v>471</v>
+        <v>492</v>
       </c>
       <c r="B20" s="106">
         <f>$B$8</f>
-        <v>87.5</v>
+        <v>12.5</v>
       </c>
       <c r="C20" s="107" t="s">
         <v>31</v>
@@ -10671,13 +10679,13 @@
         <v>366</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="21" spans="1:5" s="30" customFormat="1">
       <c r="A21" s="93" t="s">
-        <v>472</v>
+        <v>493</v>
       </c>
       <c r="B21" s="106">
         <f>$B$8</f>
-        <v>87.5</v>
+        <v>12.5</v>
       </c>
       <c r="C21" s="107" t="s">
         <v>31</v>
@@ -10689,13 +10697,13 @@
         <v>367</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="22" spans="1:5" s="30" customFormat="1">
       <c r="A22" s="93" t="s">
-        <v>473</v>
+        <v>494</v>
       </c>
       <c r="B22" s="106">
         <f>$B$8</f>
-        <v>87.5</v>
+        <v>12.5</v>
       </c>
       <c r="C22" s="107" t="s">
         <v>31</v>
@@ -10707,9 +10715,9 @@
         <v>368</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="23" spans="1:5" s="30" customFormat="1">
       <c r="A23" s="93" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B23" s="106">
         <v>100</v>
@@ -10724,9 +10732,9 @@
         <v>369</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="24" spans="1:5" s="30" customFormat="1">
       <c r="A24" s="93" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B24" s="97">
         <v>4</v>
@@ -10741,9 +10749,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="25" spans="1:5" s="30" customFormat="1">
       <c r="A25" s="94" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B25" s="98">
         <v>100</v>
@@ -10758,9 +10766,9 @@
         <v>403</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="26" spans="1:5" s="30" customFormat="1">
       <c r="A26" s="94" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B26" s="98">
         <v>100</v>
@@ -10775,9 +10783,9 @@
         <v>404</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="27" spans="1:5" s="30" customFormat="1">
       <c r="A27" s="94" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B27" s="98">
         <f>$B$4</f>
@@ -10793,9 +10801,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="30" customFormat="1" ht="17">
+    <row r="28" spans="1:5" s="30" customFormat="1">
       <c r="A28" s="94" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B28" s="98">
         <f>$B$4</f>

</xml_diff>